<commit_message>
ran discriptive statistics categorical code
</commit_message>
<xml_diff>
--- a/Descriptive Statistics/Categorical/Target_Type_summary.xlsx
+++ b/Descriptive Statistics/Categorical/Target_Type_summary.xlsx
@@ -457,10 +457,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>276</v>
+        <v>264</v>
       </c>
       <c r="C2" t="n">
-        <v>95.5</v>
+        <v>91.34999999999999</v>
       </c>
     </row>
     <row r="3">
@@ -470,10 +470,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="C3" t="n">
-        <v>4.5</v>
+        <v>8.65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>